<commit_message>
printTeamOptions function now returns the team names, not the indeces. And other changes
</commit_message>
<xml_diff>
--- a/SoccerPredictor/Soccer Points Database.xlsx
+++ b/SoccerPredictor/Soccer Points Database.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -113,14 +113,13 @@
     <t>Final rating out of 100</t>
   </si>
   <si>
-    <t>AFC Bournemouth</t>
+    <t>Bournemouth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -531,12 +530,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.08984375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.36328125" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.08984375" collapsed="true"/>
+    <col min="1" max="1" width="28.08984375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.36328125" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.08984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -1216,12 +1215,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.08984375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.36328125" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.08984375" collapsed="true"/>
+    <col min="1" max="1" width="28.08984375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.36328125" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.08984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -1266,7 +1265,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>Table2[[#This Row],[Team Name]]</f>
-        <v>AFC Bournemouth</v>
+        <v>Bournemouth</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1915,20 +1914,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.6328125" collapsed="true"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.6328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f>'2015-16'!A3</f>
-        <v>AFC Bournemouth</v>
+        <v>Bournemouth</v>
       </c>
       <c r="C1">
         <f>(1*'2015-16'!I3)+(0.5*'2014-15'!I3)</f>

</xml_diff>